<commit_message>
Arreglo y limpiado de tabla personalizada
</commit_message>
<xml_diff>
--- a/resultados/modelo_2_06.xlsx
+++ b/resultados/modelo_2_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,288 +434,1171 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>TOTAL</t>
+          <t>E. Infantil - Primer ciclo</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>E. Infantil - Primer ciclo</t>
+          <t>E. Infantil - Segundo ciclo</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>E. Infantil - Segundo ciclo</t>
+          <t>E. Primaria</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>E. Primaria</t>
+          <t>Educación Especial</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Educación Especial</t>
+          <t>ESO</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>ESO</t>
+          <t>Bachillerato</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>Bachillerato</t>
+          <t>Bachillerato a distancia</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Bachillerato a distancia</t>
+          <t>CF Grado Básico</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>CF Grado Básico</t>
+          <t>CF Grado Medio</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>CF Grado Medio</t>
+          <t>CF Grado Medio a distancia</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>CF Grado Medio a distancia</t>
+          <t>Cursos de Especialización Grado Medio</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Cursos de Especialización Grado Medio</t>
+          <t>Cursos de Especialización Grado Medio a distancia</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Cursos de Especialización Grado Medio a distancia</t>
+          <t>CF Grado Superior</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>CF Grado Superior</t>
+          <t>CF Grado Superior a distancia</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>CF Grado Superior a distancia</t>
+          <t>Cursos de Especialización Grado Superior</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Cursos de Especialización Grado Superior</t>
+          <t>Cursos de Especialización Grado Superior a distancia</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Cursos de Especialización Grado Superior a distancia</t>
+          <t>Otros Programas Formativos</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Otros Programas Formativos</t>
+          <t>Sección</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Subsección</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>01 ANDALUCÍA</t>
         </is>
       </c>
+      <c r="B2" t="n">
+        <v>1603826</v>
+      </c>
       <c r="C2" t="n">
-        <v>1603826</v>
+        <v>106619</v>
       </c>
       <c r="D2" t="n">
-        <v>106619</v>
+        <v>221323</v>
       </c>
       <c r="E2" t="n">
-        <v>221323</v>
+        <v>531221</v>
       </c>
       <c r="F2" t="n">
-        <v>531221</v>
+        <v>9426</v>
       </c>
       <c r="G2" t="n">
-        <v>9426</v>
+        <v>411932</v>
       </c>
       <c r="H2" t="n">
-        <v>411932</v>
+        <v>125265</v>
       </c>
       <c r="I2" t="n">
-        <v>125265</v>
+        <v>8537</v>
       </c>
       <c r="J2" t="n">
-        <v>8537</v>
+        <v>14482</v>
       </c>
       <c r="K2" t="n">
-        <v>14482</v>
+        <v>73480</v>
       </c>
       <c r="L2" t="n">
-        <v>73480</v>
+        <v>3342</v>
       </c>
       <c r="M2" t="n">
-        <v>3342</v>
+        <v>154</v>
       </c>
       <c r="N2" t="n">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
-        <v>0</v>
+        <v>79079</v>
       </c>
       <c r="P2" t="n">
-        <v>79079</v>
+        <v>17575</v>
       </c>
       <c r="Q2" t="n">
-        <v>17575</v>
+        <v>888</v>
       </c>
       <c r="R2" t="n">
-        <v>888</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
         <v>503</v>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>TODOS LOS CENTROS</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>AMBOS SEXOS</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>01 ANDALUCÍA</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>824964</v>
+      </c>
       <c r="C3" t="n">
-        <v>824964</v>
+        <v>55414</v>
       </c>
       <c r="D3" t="n">
-        <v>55414</v>
+        <v>113556</v>
       </c>
       <c r="E3" t="n">
-        <v>113556</v>
+        <v>273456</v>
       </c>
       <c r="F3" t="n">
-        <v>273456</v>
+        <v>6306</v>
       </c>
       <c r="G3" t="n">
-        <v>6306</v>
+        <v>212135</v>
       </c>
       <c r="H3" t="n">
-        <v>212135</v>
+        <v>57897</v>
       </c>
       <c r="I3" t="n">
-        <v>57897</v>
+        <v>4420</v>
       </c>
       <c r="J3" t="n">
-        <v>4420</v>
+        <v>10370</v>
       </c>
       <c r="K3" t="n">
-        <v>10370</v>
+        <v>40959</v>
       </c>
       <c r="L3" t="n">
-        <v>40959</v>
+        <v>1111</v>
       </c>
       <c r="M3" t="n">
-        <v>1111</v>
+        <v>130</v>
       </c>
       <c r="N3" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>40668</v>
       </c>
       <c r="P3" t="n">
-        <v>40668</v>
+        <v>7511</v>
       </c>
       <c r="Q3" t="n">
-        <v>7511</v>
+        <v>712</v>
       </c>
       <c r="R3" t="n">
-        <v>712</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" t="n">
         <v>319</v>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>TODOS LOS CENTROS</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>Hombres</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>01 ANDALUCÍA</t>
         </is>
       </c>
+      <c r="B4" t="n">
+        <v>778862</v>
+      </c>
       <c r="C4" t="n">
-        <v>778862</v>
+        <v>51205</v>
       </c>
       <c r="D4" t="n">
-        <v>51205</v>
+        <v>107767</v>
       </c>
       <c r="E4" t="n">
-        <v>107767</v>
+        <v>257765</v>
       </c>
       <c r="F4" t="n">
-        <v>257765</v>
+        <v>3120</v>
       </c>
       <c r="G4" t="n">
-        <v>3120</v>
+        <v>199797</v>
       </c>
       <c r="H4" t="n">
-        <v>199797</v>
+        <v>67368</v>
       </c>
       <c r="I4" t="n">
-        <v>67368</v>
+        <v>4117</v>
       </c>
       <c r="J4" t="n">
+        <v>4112</v>
+      </c>
+      <c r="K4" t="n">
+        <v>32521</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2231</v>
+      </c>
+      <c r="M4" t="n">
+        <v>24</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>38411</v>
+      </c>
+      <c r="P4" t="n">
+        <v>10064</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>176</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>184</v>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>TODOS LOS CENTROS</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>Mujeres</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1155976</v>
+      </c>
+      <c r="C5" t="n">
+        <v>38467</v>
+      </c>
+      <c r="D5" t="n">
+        <v>166760</v>
+      </c>
+      <c r="E5" t="n">
+        <v>401713</v>
+      </c>
+      <c r="F5" t="n">
+        <v>6770</v>
+      </c>
+      <c r="G5" t="n">
+        <v>312903</v>
+      </c>
+      <c r="H5" t="n">
+        <v>99284</v>
+      </c>
+      <c r="I5" t="n">
+        <v>8537</v>
+      </c>
+      <c r="J5" t="n">
+        <v>11010</v>
+      </c>
+      <c r="K5" t="n">
+        <v>48284</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1260</v>
+      </c>
+      <c r="M5" t="n">
+        <v>154</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>51219</v>
+      </c>
+      <c r="P5" t="n">
+        <v>8238</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>874</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>503</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>AMBOS SEXOS</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>598394</v>
+      </c>
+      <c r="C6" t="n">
+        <v>20130</v>
+      </c>
+      <c r="D6" t="n">
+        <v>85851</v>
+      </c>
+      <c r="E6" t="n">
+        <v>207661</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4563</v>
+      </c>
+      <c r="G6" t="n">
+        <v>161791</v>
+      </c>
+      <c r="H6" t="n">
+        <v>45483</v>
+      </c>
+      <c r="I6" t="n">
+        <v>4420</v>
+      </c>
+      <c r="J6" t="n">
+        <v>7989</v>
+      </c>
+      <c r="K6" t="n">
+        <v>28211</v>
+      </c>
+      <c r="L6" t="n">
+        <v>414</v>
+      </c>
+      <c r="M6" t="n">
+        <v>130</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>27349</v>
+      </c>
+      <c r="P6" t="n">
+        <v>3381</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>702</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>319</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>Hombres</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>557582</v>
+      </c>
+      <c r="C7" t="n">
+        <v>18337</v>
+      </c>
+      <c r="D7" t="n">
+        <v>80909</v>
+      </c>
+      <c r="E7" t="n">
+        <v>194052</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2207</v>
+      </c>
+      <c r="G7" t="n">
+        <v>151112</v>
+      </c>
+      <c r="H7" t="n">
+        <v>53801</v>
+      </c>
+      <c r="I7" t="n">
         <v>4117</v>
       </c>
-      <c r="K4" t="n">
+      <c r="J7" t="n">
+        <v>3021</v>
+      </c>
+      <c r="K7" t="n">
+        <v>20073</v>
+      </c>
+      <c r="L7" t="n">
+        <v>846</v>
+      </c>
+      <c r="M7" t="n">
+        <v>24</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>23870</v>
+      </c>
+      <c r="P7" t="n">
+        <v>4857</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>172</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>184</v>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>Mujeres</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>447850</v>
+      </c>
+      <c r="C8" t="n">
+        <v>68152</v>
+      </c>
+      <c r="D8" t="n">
+        <v>54563</v>
+      </c>
+      <c r="E8" t="n">
+        <v>129508</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2656</v>
+      </c>
+      <c r="G8" t="n">
+        <v>99029</v>
+      </c>
+      <c r="H8" t="n">
+        <v>25981</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>3472</v>
+      </c>
+      <c r="K8" t="n">
+        <v>25196</v>
+      </c>
+      <c r="L8" t="n">
+        <v>2082</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>27860</v>
+      </c>
+      <c r="P8" t="n">
+        <v>9337</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>14</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>Mujeres</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>226570</v>
+      </c>
+      <c r="C9" t="n">
+        <v>35284</v>
+      </c>
+      <c r="D9" t="n">
+        <v>27705</v>
+      </c>
+      <c r="E9" t="n">
+        <v>65795</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1743</v>
+      </c>
+      <c r="G9" t="n">
+        <v>50344</v>
+      </c>
+      <c r="H9" t="n">
+        <v>12414</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2381</v>
+      </c>
+      <c r="K9" t="n">
+        <v>12748</v>
+      </c>
+      <c r="L9" t="n">
+        <v>697</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>13319</v>
+      </c>
+      <c r="P9" t="n">
+        <v>4130</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>10</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>Mujeres</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>221280</v>
+      </c>
+      <c r="C10" t="n">
+        <v>32868</v>
+      </c>
+      <c r="D10" t="n">
+        <v>26858</v>
+      </c>
+      <c r="E10" t="n">
+        <v>63713</v>
+      </c>
+      <c r="F10" t="n">
+        <v>913</v>
+      </c>
+      <c r="G10" t="n">
+        <v>48685</v>
+      </c>
+      <c r="H10" t="n">
+        <v>13567</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1091</v>
+      </c>
+      <c r="K10" t="n">
+        <v>12448</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1385</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>14541</v>
+      </c>
+      <c r="P10" t="n">
+        <v>5207</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>4</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>Mujeres</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>336075</v>
+      </c>
+      <c r="C11" t="n">
+        <v>61432</v>
+      </c>
+      <c r="D11" t="n">
+        <v>46167</v>
+      </c>
+      <c r="E11" t="n">
+        <v>108772</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2652</v>
+      </c>
+      <c r="G11" t="n">
+        <v>82399</v>
+      </c>
+      <c r="H11" t="n">
+        <v>7635</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>3429</v>
+      </c>
+      <c r="K11" t="n">
+        <v>16755</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>6834</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>Mujeres</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>171913</v>
+      </c>
+      <c r="C12" t="n">
+        <v>31805</v>
+      </c>
+      <c r="D12" t="n">
+        <v>23387</v>
+      </c>
+      <c r="E12" t="n">
+        <v>55248</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1742</v>
+      </c>
+      <c r="G12" t="n">
+        <v>41906</v>
+      </c>
+      <c r="H12" t="n">
+        <v>3662</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2339</v>
+      </c>
+      <c r="K12" t="n">
+        <v>8419</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>3405</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>Mujeres</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>164162</v>
+      </c>
+      <c r="C13" t="n">
+        <v>29627</v>
+      </c>
+      <c r="D13" t="n">
+        <v>22780</v>
+      </c>
+      <c r="E13" t="n">
+        <v>53524</v>
+      </c>
+      <c r="F13" t="n">
+        <v>910</v>
+      </c>
+      <c r="G13" t="n">
+        <v>40493</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3973</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1090</v>
+      </c>
+      <c r="K13" t="n">
+        <v>8336</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>3429</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>Mujeres</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>111775</v>
+      </c>
+      <c r="C14" t="n">
+        <v>6720</v>
+      </c>
+      <c r="D14" t="n">
+        <v>8396</v>
+      </c>
+      <c r="E14" t="n">
+        <v>20736</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4</v>
+      </c>
+      <c r="G14" t="n">
+        <v>16630</v>
+      </c>
+      <c r="H14" t="n">
+        <v>18346</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>43</v>
+      </c>
+      <c r="K14" t="n">
+        <v>8441</v>
+      </c>
+      <c r="L14" t="n">
+        <v>2082</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>21026</v>
+      </c>
+      <c r="P14" t="n">
+        <v>9337</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>14</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>Mujeres</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>54657</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3479</v>
+      </c>
+      <c r="D15" t="n">
+        <v>4318</v>
+      </c>
+      <c r="E15" t="n">
+        <v>10547</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>8438</v>
+      </c>
+      <c r="H15" t="n">
+        <v>8752</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>42</v>
+      </c>
+      <c r="K15" t="n">
+        <v>4329</v>
+      </c>
+      <c r="L15" t="n">
+        <v>697</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>9914</v>
+      </c>
+      <c r="P15" t="n">
+        <v>4130</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>10</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>Mujeres</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>01 ANDALUCÍA</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>57118</v>
+      </c>
+      <c r="C16" t="n">
+        <v>3241</v>
+      </c>
+      <c r="D16" t="n">
+        <v>4078</v>
+      </c>
+      <c r="E16" t="n">
+        <v>10189</v>
+      </c>
+      <c r="F16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" t="n">
+        <v>8192</v>
+      </c>
+      <c r="H16" t="n">
+        <v>9594</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
         <v>4112</v>
       </c>
-      <c r="L4" t="n">
-        <v>32521</v>
-      </c>
-      <c r="M4" t="n">
-        <v>2231</v>
-      </c>
-      <c r="N4" t="n">
-        <v>24</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>38411</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>10064</v>
-      </c>
-      <c r="R4" t="n">
-        <v>176</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" t="n">
-        <v>184</v>
+      <c r="L16" t="n">
+        <v>1385</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>11112</v>
+      </c>
+      <c r="P16" t="n">
+        <v>5207</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>4</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>Mujeres</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Limpieza y arreglo de interfaz
</commit_message>
<xml_diff>
--- a/resultados/modelo_2_06.xlsx
+++ b/resultados/modelo_2_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -527,10 +527,15 @@
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
+          <t>Archivo</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
           <t>Sección</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Subsección</t>
         </is>
@@ -598,10 +603,15 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
+          <t>regimen_general.xls</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
           <t>TODOS LOS CENTROS</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="V2" t="inlineStr">
         <is>
           <t>AMBOS SEXOS</t>
         </is>
@@ -669,10 +679,15 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
+          <t>regimen_general.xls</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
           <t>TODOS LOS CENTROS</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="V3" t="inlineStr">
         <is>
           <t>Hombres</t>
         </is>
@@ -740,12 +755,17 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
+          <t>regimen_general.xls</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
           <t>TODOS LOS CENTROS</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Mujeres</t>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>Hombres</t>
         </is>
       </c>
     </row>
@@ -756,65 +776,70 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1155976</v>
+        <v>447850</v>
       </c>
       <c r="C5" t="n">
-        <v>38467</v>
+        <v>68152</v>
       </c>
       <c r="D5" t="n">
-        <v>166760</v>
+        <v>54563</v>
       </c>
       <c r="E5" t="n">
-        <v>401713</v>
+        <v>129508</v>
       </c>
       <c r="F5" t="n">
-        <v>6770</v>
+        <v>2656</v>
       </c>
       <c r="G5" t="n">
-        <v>312903</v>
+        <v>99029</v>
       </c>
       <c r="H5" t="n">
-        <v>99284</v>
+        <v>25981</v>
       </c>
       <c r="I5" t="n">
-        <v>8537</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>11010</v>
+        <v>3472</v>
       </c>
       <c r="K5" t="n">
-        <v>48284</v>
+        <v>25196</v>
       </c>
       <c r="L5" t="n">
-        <v>1260</v>
+        <v>2082</v>
       </c>
       <c r="M5" t="n">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
       </c>
       <c r="O5" t="n">
-        <v>51219</v>
+        <v>27860</v>
       </c>
       <c r="P5" t="n">
-        <v>8238</v>
+        <v>9337</v>
       </c>
       <c r="Q5" t="n">
-        <v>874</v>
+        <v>14</v>
       </c>
       <c r="R5" t="n">
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>503</v>
+        <v>0</v>
       </c>
       <c r="T5" t="inlineStr">
         <is>
+          <t>regimen_general.xls</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
           <t>CENTROS PÚBLICOS</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="V5" t="inlineStr">
         <is>
           <t>AMBOS SEXOS</t>
         </is>
@@ -827,65 +852,70 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>598394</v>
+        <v>226570</v>
       </c>
       <c r="C6" t="n">
-        <v>20130</v>
+        <v>35284</v>
       </c>
       <c r="D6" t="n">
-        <v>85851</v>
+        <v>27705</v>
       </c>
       <c r="E6" t="n">
-        <v>207661</v>
+        <v>65795</v>
       </c>
       <c r="F6" t="n">
-        <v>4563</v>
+        <v>1743</v>
       </c>
       <c r="G6" t="n">
-        <v>161791</v>
+        <v>50344</v>
       </c>
       <c r="H6" t="n">
-        <v>45483</v>
+        <v>12414</v>
       </c>
       <c r="I6" t="n">
-        <v>4420</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>7989</v>
+        <v>2381</v>
       </c>
       <c r="K6" t="n">
-        <v>28211</v>
+        <v>12748</v>
       </c>
       <c r="L6" t="n">
-        <v>414</v>
+        <v>697</v>
       </c>
       <c r="M6" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
       </c>
       <c r="O6" t="n">
-        <v>27349</v>
+        <v>13319</v>
       </c>
       <c r="P6" t="n">
-        <v>3381</v>
+        <v>4130</v>
       </c>
       <c r="Q6" t="n">
-        <v>702</v>
+        <v>10</v>
       </c>
       <c r="R6" t="n">
         <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>319</v>
+        <v>0</v>
       </c>
       <c r="T6" t="inlineStr">
         <is>
+          <t>regimen_general.xls</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
           <t>CENTROS PÚBLICOS</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr">
+      <c r="V6" t="inlineStr">
         <is>
           <t>Hombres</t>
         </is>
@@ -898,704 +928,70 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>557582</v>
+        <v>221280</v>
       </c>
       <c r="C7" t="n">
-        <v>18337</v>
+        <v>32868</v>
       </c>
       <c r="D7" t="n">
-        <v>80909</v>
+        <v>26858</v>
       </c>
       <c r="E7" t="n">
-        <v>194052</v>
+        <v>63713</v>
       </c>
       <c r="F7" t="n">
-        <v>2207</v>
+        <v>913</v>
       </c>
       <c r="G7" t="n">
-        <v>151112</v>
+        <v>48685</v>
       </c>
       <c r="H7" t="n">
-        <v>53801</v>
+        <v>13567</v>
       </c>
       <c r="I7" t="n">
-        <v>4117</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>3021</v>
+        <v>1091</v>
       </c>
       <c r="K7" t="n">
-        <v>20073</v>
+        <v>12448</v>
       </c>
       <c r="L7" t="n">
-        <v>846</v>
+        <v>1385</v>
       </c>
       <c r="M7" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
       </c>
       <c r="O7" t="n">
-        <v>23870</v>
+        <v>14541</v>
       </c>
       <c r="P7" t="n">
-        <v>4857</v>
+        <v>5207</v>
       </c>
       <c r="Q7" t="n">
-        <v>172</v>
+        <v>4</v>
       </c>
       <c r="R7" t="n">
         <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>184</v>
+        <v>0</v>
       </c>
       <c r="T7" t="inlineStr">
         <is>
+          <t>regimen_general.xls</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
           <t>CENTROS PÚBLICOS</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>Mujeres</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>01 ANDALUCÍA</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>447850</v>
-      </c>
-      <c r="C8" t="n">
-        <v>68152</v>
-      </c>
-      <c r="D8" t="n">
-        <v>54563</v>
-      </c>
-      <c r="E8" t="n">
-        <v>129508</v>
-      </c>
-      <c r="F8" t="n">
-        <v>2656</v>
-      </c>
-      <c r="G8" t="n">
-        <v>99029</v>
-      </c>
-      <c r="H8" t="n">
-        <v>25981</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>3472</v>
-      </c>
-      <c r="K8" t="n">
-        <v>25196</v>
-      </c>
-      <c r="L8" t="n">
-        <v>2082</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" t="n">
-        <v>27860</v>
-      </c>
-      <c r="P8" t="n">
-        <v>9337</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>14</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>CENTROS PÚBLICOS</t>
-        </is>
-      </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>Mujeres</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>01 ANDALUCÍA</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>226570</v>
-      </c>
-      <c r="C9" t="n">
-        <v>35284</v>
-      </c>
-      <c r="D9" t="n">
-        <v>27705</v>
-      </c>
-      <c r="E9" t="n">
-        <v>65795</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1743</v>
-      </c>
-      <c r="G9" t="n">
-        <v>50344</v>
-      </c>
-      <c r="H9" t="n">
-        <v>12414</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>2381</v>
-      </c>
-      <c r="K9" t="n">
-        <v>12748</v>
-      </c>
-      <c r="L9" t="n">
-        <v>697</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
-        <v>13319</v>
-      </c>
-      <c r="P9" t="n">
-        <v>4130</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>10</v>
-      </c>
-      <c r="R9" t="n">
-        <v>0</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0</v>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>CENTROS PÚBLICOS</t>
-        </is>
-      </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>Mujeres</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>01 ANDALUCÍA</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>221280</v>
-      </c>
-      <c r="C10" t="n">
-        <v>32868</v>
-      </c>
-      <c r="D10" t="n">
-        <v>26858</v>
-      </c>
-      <c r="E10" t="n">
-        <v>63713</v>
-      </c>
-      <c r="F10" t="n">
-        <v>913</v>
-      </c>
-      <c r="G10" t="n">
-        <v>48685</v>
-      </c>
-      <c r="H10" t="n">
-        <v>13567</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>1091</v>
-      </c>
-      <c r="K10" t="n">
-        <v>12448</v>
-      </c>
-      <c r="L10" t="n">
-        <v>1385</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="n">
-        <v>14541</v>
-      </c>
-      <c r="P10" t="n">
-        <v>5207</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>4</v>
-      </c>
-      <c r="R10" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" t="n">
-        <v>0</v>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>CENTROS PÚBLICOS</t>
-        </is>
-      </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>Mujeres</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>01 ANDALUCÍA</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>336075</v>
-      </c>
-      <c r="C11" t="n">
-        <v>61432</v>
-      </c>
-      <c r="D11" t="n">
-        <v>46167</v>
-      </c>
-      <c r="E11" t="n">
-        <v>108772</v>
-      </c>
-      <c r="F11" t="n">
-        <v>2652</v>
-      </c>
-      <c r="G11" t="n">
-        <v>82399</v>
-      </c>
-      <c r="H11" t="n">
-        <v>7635</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>3429</v>
-      </c>
-      <c r="K11" t="n">
-        <v>16755</v>
-      </c>
-      <c r="L11" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" t="n">
-        <v>6834</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" t="n">
-        <v>0</v>
-      </c>
-      <c r="S11" t="n">
-        <v>0</v>
-      </c>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>CENTROS PÚBLICOS</t>
-        </is>
-      </c>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>Mujeres</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>01 ANDALUCÍA</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>171913</v>
-      </c>
-      <c r="C12" t="n">
-        <v>31805</v>
-      </c>
-      <c r="D12" t="n">
-        <v>23387</v>
-      </c>
-      <c r="E12" t="n">
-        <v>55248</v>
-      </c>
-      <c r="F12" t="n">
-        <v>1742</v>
-      </c>
-      <c r="G12" t="n">
-        <v>41906</v>
-      </c>
-      <c r="H12" t="n">
-        <v>3662</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>2339</v>
-      </c>
-      <c r="K12" t="n">
-        <v>8419</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>3405</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" t="n">
-        <v>0</v>
-      </c>
-      <c r="S12" t="n">
-        <v>0</v>
-      </c>
-      <c r="T12" t="inlineStr">
-        <is>
-          <t>CENTROS PÚBLICOS</t>
-        </is>
-      </c>
-      <c r="U12" t="inlineStr">
-        <is>
-          <t>Mujeres</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>01 ANDALUCÍA</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>164162</v>
-      </c>
-      <c r="C13" t="n">
-        <v>29627</v>
-      </c>
-      <c r="D13" t="n">
-        <v>22780</v>
-      </c>
-      <c r="E13" t="n">
-        <v>53524</v>
-      </c>
-      <c r="F13" t="n">
-        <v>910</v>
-      </c>
-      <c r="G13" t="n">
-        <v>40493</v>
-      </c>
-      <c r="H13" t="n">
-        <v>3973</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>1090</v>
-      </c>
-      <c r="K13" t="n">
-        <v>8336</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" t="n">
-        <v>3429</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" t="n">
-        <v>0</v>
-      </c>
-      <c r="S13" t="n">
-        <v>0</v>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>CENTROS PÚBLICOS</t>
-        </is>
-      </c>
-      <c r="U13" t="inlineStr">
-        <is>
-          <t>Mujeres</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>01 ANDALUCÍA</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>111775</v>
-      </c>
-      <c r="C14" t="n">
-        <v>6720</v>
-      </c>
-      <c r="D14" t="n">
-        <v>8396</v>
-      </c>
-      <c r="E14" t="n">
-        <v>20736</v>
-      </c>
-      <c r="F14" t="n">
-        <v>4</v>
-      </c>
-      <c r="G14" t="n">
-        <v>16630</v>
-      </c>
-      <c r="H14" t="n">
-        <v>18346</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>43</v>
-      </c>
-      <c r="K14" t="n">
-        <v>8441</v>
-      </c>
-      <c r="L14" t="n">
-        <v>2082</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="n">
-        <v>21026</v>
-      </c>
-      <c r="P14" t="n">
-        <v>9337</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>14</v>
-      </c>
-      <c r="R14" t="n">
-        <v>0</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0</v>
-      </c>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>CENTROS PÚBLICOS</t>
-        </is>
-      </c>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>Mujeres</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>01 ANDALUCÍA</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>54657</v>
-      </c>
-      <c r="C15" t="n">
-        <v>3479</v>
-      </c>
-      <c r="D15" t="n">
-        <v>4318</v>
-      </c>
-      <c r="E15" t="n">
-        <v>10547</v>
-      </c>
-      <c r="F15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" t="n">
-        <v>8438</v>
-      </c>
-      <c r="H15" t="n">
-        <v>8752</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>42</v>
-      </c>
-      <c r="K15" t="n">
-        <v>4329</v>
-      </c>
-      <c r="L15" t="n">
-        <v>697</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
-        <v>9914</v>
-      </c>
-      <c r="P15" t="n">
-        <v>4130</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>10</v>
-      </c>
-      <c r="R15" t="n">
-        <v>0</v>
-      </c>
-      <c r="S15" t="n">
-        <v>0</v>
-      </c>
-      <c r="T15" t="inlineStr">
-        <is>
-          <t>CENTROS PÚBLICOS</t>
-        </is>
-      </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>Mujeres</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>01 ANDALUCÍA</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>57118</v>
-      </c>
-      <c r="C16" t="n">
-        <v>3241</v>
-      </c>
-      <c r="D16" t="n">
-        <v>4078</v>
-      </c>
-      <c r="E16" t="n">
-        <v>10189</v>
-      </c>
-      <c r="F16" t="n">
-        <v>3</v>
-      </c>
-      <c r="G16" t="n">
-        <v>8192</v>
-      </c>
-      <c r="H16" t="n">
-        <v>9594</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" t="n">
-        <v>4112</v>
-      </c>
-      <c r="L16" t="n">
-        <v>1385</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" t="n">
-        <v>11112</v>
-      </c>
-      <c r="P16" t="n">
-        <v>5207</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>4</v>
-      </c>
-      <c r="R16" t="n">
-        <v>0</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0</v>
-      </c>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>CENTROS PÚBLICOS</t>
-        </is>
-      </c>
-      <c r="U16" t="inlineStr">
+      <c r="V7" t="inlineStr">
         <is>
           <t>Mujeres</t>
         </is>

</xml_diff>

<commit_message>
Implementación de sección y subsección en excel resultante (+arreglo pánico git)
</commit_message>
<xml_diff>
--- a/resultados/modelo_2_06.xlsx
+++ b/resultados/modelo_2_06.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,567 +434,536 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sección</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Subsección</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Fila</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>E. Infantil - Primer ciclo</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>E. Infantil - Segundo ciclo</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>E. Primaria</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Educación Especial</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>ESO</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Bachillerato</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Bachillerato a distancia</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>CF Grado Básico</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>CF Grado Medio</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>CF Grado Medio a distancia</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Cursos de Especialización Grado Medio</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Cursos de Especialización Grado Medio a distancia</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>CF Grado Superior</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>CF Grado Superior a distancia</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Cursos de Especialización Grado Superior</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Cursos de Especialización Grado Superior a distancia</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Otros Programas Formativos</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Archivo</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Sección</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>Subsección</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>TODOS LOS CENTROS</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AMBOS SEXOS</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>01 ANDALUCÍA</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="D2" t="n">
         <v>1603826</v>
       </c>
-      <c r="C2" t="n">
+      <c r="E2" t="n">
         <v>106619</v>
       </c>
-      <c r="D2" t="n">
+      <c r="F2" t="n">
         <v>221323</v>
       </c>
-      <c r="E2" t="n">
+      <c r="G2" t="n">
         <v>531221</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>9426</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>411932</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>125265</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>8537</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>14482</v>
       </c>
-      <c r="K2" t="n">
+      <c r="M2" t="n">
         <v>73480</v>
       </c>
-      <c r="L2" t="n">
+      <c r="N2" t="n">
         <v>3342</v>
       </c>
-      <c r="M2" t="n">
+      <c r="O2" t="n">
         <v>154</v>
       </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
         <v>79079</v>
       </c>
-      <c r="P2" t="n">
+      <c r="R2" t="n">
         <v>17575</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="S2" t="n">
         <v>888</v>
       </c>
-      <c r="R2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
         <v>503</v>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>regimen_general.xls</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>TODOS LOS CENTROS</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>AMBOS SEXOS</t>
-        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>TODOS LOS CENTROS</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Hombres</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>01 ANDALUCÍA</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="D3" t="n">
         <v>824964</v>
       </c>
-      <c r="C3" t="n">
+      <c r="E3" t="n">
         <v>55414</v>
       </c>
-      <c r="D3" t="n">
+      <c r="F3" t="n">
         <v>113556</v>
       </c>
-      <c r="E3" t="n">
+      <c r="G3" t="n">
         <v>273456</v>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
         <v>6306</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>212135</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>57897</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>4420</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
         <v>10370</v>
       </c>
-      <c r="K3" t="n">
+      <c r="M3" t="n">
         <v>40959</v>
       </c>
-      <c r="L3" t="n">
+      <c r="N3" t="n">
         <v>1111</v>
       </c>
-      <c r="M3" t="n">
+      <c r="O3" t="n">
         <v>130</v>
       </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
         <v>40668</v>
       </c>
-      <c r="P3" t="n">
+      <c r="R3" t="n">
         <v>7511</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="S3" t="n">
         <v>712</v>
       </c>
-      <c r="R3" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
         <v>319</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>regimen_general.xls</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>TODOS LOS CENTROS</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>Hombres</t>
-        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>TODOS LOS CENTROS</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Mujeres</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>01 ANDALUCÍA</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="D4" t="n">
         <v>778862</v>
       </c>
-      <c r="C4" t="n">
+      <c r="E4" t="n">
         <v>51205</v>
       </c>
-      <c r="D4" t="n">
+      <c r="F4" t="n">
         <v>107767</v>
       </c>
-      <c r="E4" t="n">
+      <c r="G4" t="n">
         <v>257765</v>
       </c>
-      <c r="F4" t="n">
+      <c r="H4" t="n">
         <v>3120</v>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" t="n">
         <v>199797</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>67368</v>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
         <v>4117</v>
       </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
         <v>4112</v>
       </c>
-      <c r="K4" t="n">
+      <c r="M4" t="n">
         <v>32521</v>
       </c>
-      <c r="L4" t="n">
+      <c r="N4" t="n">
         <v>2231</v>
       </c>
-      <c r="M4" t="n">
+      <c r="O4" t="n">
         <v>24</v>
       </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
         <v>38411</v>
       </c>
-      <c r="P4" t="n">
+      <c r="R4" t="n">
         <v>10064</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="S4" t="n">
         <v>176</v>
       </c>
-      <c r="R4" t="n">
-        <v>0</v>
-      </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
         <v>184</v>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>regimen_general.xls</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>TODOS LOS CENTROS</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>Hombres</t>
-        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>AMBOS SEXOS</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>01 ANDALUCÍA</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="D5" t="n">
         <v>447850</v>
       </c>
-      <c r="C5" t="n">
+      <c r="E5" t="n">
         <v>68152</v>
       </c>
-      <c r="D5" t="n">
+      <c r="F5" t="n">
         <v>54563</v>
       </c>
-      <c r="E5" t="n">
+      <c r="G5" t="n">
         <v>129508</v>
       </c>
-      <c r="F5" t="n">
+      <c r="H5" t="n">
         <v>2656</v>
       </c>
-      <c r="G5" t="n">
+      <c r="I5" t="n">
         <v>99029</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>25981</v>
       </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
         <v>3472</v>
       </c>
-      <c r="K5" t="n">
+      <c r="M5" t="n">
         <v>25196</v>
       </c>
-      <c r="L5" t="n">
+      <c r="N5" t="n">
         <v>2082</v>
       </c>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
       <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
         <v>27860</v>
       </c>
-      <c r="P5" t="n">
+      <c r="R5" t="n">
         <v>9337</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="S5" t="n">
         <v>14</v>
       </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>regimen_general.xls</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>CENTROS PÚBLICOS</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>AMBOS SEXOS</t>
-        </is>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Hombres</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>01 ANDALUCÍA</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="D6" t="n">
         <v>226570</v>
       </c>
-      <c r="C6" t="n">
+      <c r="E6" t="n">
         <v>35284</v>
       </c>
-      <c r="D6" t="n">
+      <c r="F6" t="n">
         <v>27705</v>
       </c>
-      <c r="E6" t="n">
+      <c r="G6" t="n">
         <v>65795</v>
       </c>
-      <c r="F6" t="n">
+      <c r="H6" t="n">
         <v>1743</v>
       </c>
-      <c r="G6" t="n">
+      <c r="I6" t="n">
         <v>50344</v>
       </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
         <v>12414</v>
       </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
         <v>2381</v>
       </c>
-      <c r="K6" t="n">
+      <c r="M6" t="n">
         <v>12748</v>
       </c>
-      <c r="L6" t="n">
+      <c r="N6" t="n">
         <v>697</v>
       </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
       <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
         <v>13319</v>
       </c>
-      <c r="P6" t="n">
+      <c r="R6" t="n">
         <v>4130</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="S6" t="n">
         <v>10</v>
       </c>
-      <c r="R6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>regimen_general.xls</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>CENTROS PÚBLICOS</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>Hombres</t>
-        </is>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>CENTROS PÚBLICOS</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Mujeres</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>01 ANDALUCÍA</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="D7" t="n">
         <v>221280</v>
       </c>
-      <c r="C7" t="n">
+      <c r="E7" t="n">
         <v>32868</v>
       </c>
-      <c r="D7" t="n">
+      <c r="F7" t="n">
         <v>26858</v>
       </c>
-      <c r="E7" t="n">
+      <c r="G7" t="n">
         <v>63713</v>
       </c>
-      <c r="F7" t="n">
+      <c r="H7" t="n">
         <v>913</v>
       </c>
-      <c r="G7" t="n">
+      <c r="I7" t="n">
         <v>48685</v>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
         <v>13567</v>
       </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
         <v>1091</v>
       </c>
-      <c r="K7" t="n">
+      <c r="M7" t="n">
         <v>12448</v>
       </c>
-      <c r="L7" t="n">
+      <c r="N7" t="n">
         <v>1385</v>
       </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
       <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
         <v>14541</v>
       </c>
-      <c r="P7" t="n">
+      <c r="R7" t="n">
         <v>5207</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="S7" t="n">
         <v>4</v>
       </c>
-      <c r="R7" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0</v>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>regimen_general.xls</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>CENTROS PÚBLICOS</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>Mujeres</t>
-        </is>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>